<commit_message>
29 agustus 2019 titik darah penghabisan
</commit_message>
<xml_diff>
--- a/carimobil.xlsx
+++ b/carimobil.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>brand</t>
   </si>
@@ -62,25 +62,37 @@
     <t>terbuka</t>
   </si>
   <si>
-    <t>ferrari</t>
-  </si>
-  <si>
-    <t>spider</t>
-  </si>
-  <si>
-    <t>f 430 coupe</t>
-  </si>
-  <si>
-    <t>manual</t>
-  </si>
-  <si>
-    <t>tertutup</t>
-  </si>
-  <si>
     <t>jaraktempuh</t>
   </si>
   <si>
     <t>tipelelang</t>
+  </si>
+  <si>
+    <t>expected</t>
+  </si>
+  <si>
+    <t>keterangan</t>
+  </si>
+  <si>
+    <t>passed</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>fieldempty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ferrari </t>
+  </si>
+  <si>
+    <t>795(CKD)</t>
+  </si>
+  <si>
+    <t>automatic</t>
+  </si>
+  <si>
+    <t>brandsalah</t>
   </si>
 </sst>
 </file>
@@ -398,26 +410,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
     <col min="8" max="8" width="18.42578125" customWidth="1"/>
     <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -437,16 +451,22 @@
         <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
         <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -468,28 +488,45 @@
       <c r="I2" t="s">
         <v>11</v>
       </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4">
         <v>2015</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <v>2017</v>
       </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>